<commit_message>
Added vendors and products data to xls file;
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="660" windowWidth="30560" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="22880" yWindow="2340" windowWidth="30560" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Vendors" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -41,12 +41,6 @@
     <t>Unit</t>
   </si>
   <si>
-    <t>Мин. Вода Девин 1.5л</t>
-  </si>
-  <si>
-    <t>Белла ООД</t>
-  </si>
-  <si>
     <t>бр</t>
   </si>
   <si>
@@ -56,7 +50,124 @@
     <t>литър</t>
   </si>
   <si>
-    <t>Мин Вода Девин 0.5л</t>
+    <t>Ahmad Tea</t>
+  </si>
+  <si>
+    <t>Frutelli</t>
+  </si>
+  <si>
+    <t>Lacrima</t>
+  </si>
+  <si>
+    <t>Veselina Trade OOD</t>
+  </si>
+  <si>
+    <t>Zaharni Zavodi</t>
+  </si>
+  <si>
+    <t>KFM - Karol Fernander Meat</t>
+  </si>
+  <si>
+    <t>Madjarov</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Devin JSC </t>
+  </si>
+  <si>
+    <t>Absolut Vodka - Pernaud Ricard</t>
+  </si>
+  <si>
+    <t>Wall's (Algida)</t>
+  </si>
+  <si>
+    <t>Zagorka SA</t>
+  </si>
+  <si>
+    <t>Intersnack (Chio Chips)</t>
+  </si>
+  <si>
+    <t>Coca-Cola HBC AG</t>
+  </si>
+  <si>
+    <t>Ken AD</t>
+  </si>
+  <si>
+    <t>Deroni Ltd</t>
+  </si>
+  <si>
+    <t>Olineza OOD</t>
+  </si>
+  <si>
+    <t>Luigi Lavazza S.p.A.</t>
+  </si>
+  <si>
+    <t>MEGGLE Bulgaria EOOD</t>
+  </si>
+  <si>
+    <t>Mondelez (Milka)</t>
+  </si>
+  <si>
+    <t>Min. Voda Devin 1.5</t>
+  </si>
+  <si>
+    <t>Min. Voda Devin 0.5</t>
+  </si>
+  <si>
+    <t>Absolut Vodka 1.5L</t>
+  </si>
+  <si>
+    <t>Absolut Vodka 1.0L</t>
+  </si>
+  <si>
+    <t>Absolut Wild Tea 1.0L</t>
+  </si>
+  <si>
+    <t>Ahmad Green Tea 20x2g</t>
+  </si>
+  <si>
+    <t>Ahmad Green Tea Lemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ahmad Green Tea Original </t>
+  </si>
+  <si>
+    <t>Algida Carte D'or</t>
+  </si>
+  <si>
+    <t>Algida Carte D'or Chocolate</t>
+  </si>
+  <si>
+    <t>Algida Carte D'or Cherry</t>
+  </si>
+  <si>
+    <t>Zagorka MAXX 0.5l</t>
+  </si>
+  <si>
+    <t>Zagorka 1L</t>
+  </si>
+  <si>
+    <t>Zagorka 2L</t>
+  </si>
+  <si>
+    <t>Zagorka 0.5L</t>
+  </si>
+  <si>
+    <t>PomBar</t>
+  </si>
+  <si>
+    <t>PomBar Onion &amp; Cream</t>
+  </si>
+  <si>
+    <t>Micro Popcorn 80g</t>
+  </si>
+  <si>
+    <t>Jiva Bira</t>
+  </si>
+  <si>
+    <t>Jiva Bira OOD</t>
+  </si>
+  <si>
+    <t>Lavazza Crema 250g</t>
   </si>
 </sst>
 </file>
@@ -99,9 +210,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,13 +545,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="20">
       <c r="A1" s="1" t="s">
@@ -454,17 +569,159 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -479,15 +736,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -514,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -522,7 +779,7 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>0.77</v>
       </c>
     </row>
@@ -531,16 +788,322 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45.14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>32.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>35.69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0.43</v>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2">
+        <v>8.39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2">
+        <v>2.99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="2">
+        <v>8.99</v>
       </c>
     </row>
   </sheetData>
@@ -576,7 +1139,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -584,7 +1147,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -592,7 +1155,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>